<commit_message>
bilan data set avec ai result
</commit_message>
<xml_diff>
--- a/Data_Set/Raw/Bilan-dataSet.xlsx
+++ b/Data_Set/Raw/Bilan-dataSet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnaud\Documents\École\Universite\Bio-instru\Bio_instru_2020\Data_Set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnaud\Documents\École\Universite\Bio-instru\Bio_instru_2020\Data_Set\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Nom</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Average Deviation</t>
+  </si>
+  <si>
+    <t>Model prediction</t>
   </si>
 </sst>
 </file>
@@ -381,20 +384,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,14 +420,17 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -445,16 +452,19 @@
       <c r="G2">
         <v>95.987200000000001</v>
       </c>
-      <c r="I2">
+      <c r="H2">
+        <v>94.687248093435002</v>
+      </c>
+      <c r="L2">
         <f>110-25*((E2/C2)/(F2/D2))</f>
         <v>96.012349146745905</v>
       </c>
-      <c r="J2">
-        <f>ABS(I2-G2)</f>
+      <c r="M2">
+        <f>ABS(L2-G2)</f>
         <v>2.5149146745903295E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -476,16 +486,19 @@
       <c r="G3">
         <v>94.021199999999993</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I6" si="0">110-25*((E3/C3)/(F3/D3))</f>
+      <c r="H3">
+        <v>94.959077458293095</v>
+      </c>
+      <c r="L3">
+        <f>110-25*((E3/C3)/(F3/D3))</f>
         <v>93.628005657708627</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J14" si="1">ABS(I3-G3)</f>
+      <c r="M3">
+        <f>ABS(L3-G3)</f>
         <v>0.39319434229136618</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -507,16 +520,19 @@
       <c r="G4">
         <v>64.846500000000006</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
+      <c r="H4">
+        <v>64.4323129265115</v>
+      </c>
+      <c r="L4">
+        <f>110-25*((E4/C4)/(F4/D4))</f>
         <v>52.849525696542891</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="1"/>
+      <c r="M4">
+        <f>ABS(L4-G4)</f>
         <v>11.996974303457115</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -538,16 +554,19 @@
       <c r="G5">
         <v>93.720200000000006</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
+      <c r="H5">
+        <v>94.016962524455096</v>
+      </c>
+      <c r="L5">
+        <f>110-25*((E5/C5)/(F5/D5))</f>
         <v>93.674654736176279</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
+      <c r="M5">
+        <f>ABS(L5-G5)</f>
         <v>4.5545263823726145E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -569,16 +588,19 @@
       <c r="G6">
         <v>89.3994</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
+      <c r="H6">
+        <v>87.279647474527806</v>
+      </c>
+      <c r="L6">
+        <f>110-25*((E6/C6)/(F6/D6))</f>
         <v>86.976470911999485</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
+      <c r="M6">
+        <f>ABS(L6-G6)</f>
         <v>2.4229290880005152</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -600,16 +622,19 @@
       <c r="G7">
         <v>82.846500000000006</v>
       </c>
-      <c r="I7">
+      <c r="H7">
+        <v>85.653102188874399</v>
+      </c>
+      <c r="L7">
         <f>110-25*((E7/C7)/(F7/D7))</f>
         <v>86.752771464848536</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
+      <c r="M7">
+        <f>ABS(L7-G7)</f>
         <v>3.9062714648485297</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -631,16 +656,19 @@
       <c r="G8">
         <v>81.807699999999997</v>
       </c>
-      <c r="I8">
-        <f t="shared" ref="I8:I14" si="2">110-25*((E8/C8)/(F8/D8))</f>
+      <c r="H8">
+        <v>82.359686356429293</v>
+      </c>
+      <c r="L8">
+        <f>110-25*((E8/C8)/(F8/D8))</f>
         <v>81.946816127047242</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
+      <c r="M8">
+        <f>ABS(L8-G8)</f>
         <v>0.13911612704724519</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -662,16 +690,19 @@
       <c r="G9">
         <v>85.099699999999999</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
+      <c r="H9">
+        <v>85.242444694750503</v>
+      </c>
+      <c r="L9">
+        <f>110-25*((E9/C9)/(F9/D9))</f>
         <v>81.05399121673986</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
+      <c r="M9">
+        <f>ABS(L9-G9)</f>
         <v>4.0457087832601388</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -693,16 +724,19 @@
       <c r="G10">
         <v>91.972399999999993</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
+      <c r="H10">
+        <v>89.632383875928298</v>
+      </c>
+      <c r="L10">
+        <f>110-25*((E10/C10)/(F10/D10))</f>
         <v>91.91245791245791</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
+      <c r="M10">
+        <f>ABS(L10-G10)</f>
         <v>5.99420875420833E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -724,16 +758,19 @@
       <c r="G11">
         <v>92.323599999999999</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="2"/>
+      <c r="H11">
+        <v>89.348543617324793</v>
+      </c>
+      <c r="L11">
+        <f>110-25*((E11/C11)/(F11/D11))</f>
         <v>91.184471083183325</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
+      <c r="M11">
+        <f>ABS(L11-G11)</f>
         <v>1.1391289168166736</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -755,16 +792,19 @@
       <c r="G12">
         <v>89.424300000000002</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
+      <c r="H12">
+        <v>89.566795231854002</v>
+      </c>
+      <c r="L12">
+        <f>110-25*((E12/C12)/(F12/D12))</f>
         <v>88.397307614242123</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="1"/>
+      <c r="M12">
+        <f>ABS(L12-G12)</f>
         <v>1.0269923857578789</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -786,16 +826,19 @@
       <c r="G13">
         <v>85.177300000000002</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
+      <c r="H13">
+        <v>89.590290789469705</v>
+      </c>
+      <c r="L13">
+        <f>110-25*((E13/C13)/(F13/D13))</f>
         <v>85.507562112623816</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
+      <c r="M13">
+        <f>ABS(L13-G13)</f>
         <v>0.33026211262381366</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -817,22 +860,90 @@
       <c r="G14">
         <v>94.146799999999999</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
+      <c r="H14">
+        <v>94.132884696235607</v>
+      </c>
+      <c r="L14">
+        <f>110-25*((E14/C14)/(F14/D14))</f>
         <v>91.067007878656895</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
+      <c r="M14">
+        <f>ABS(L14-G14)</f>
         <v>3.0797921213431039</v>
       </c>
     </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I23" t="s">
+    <row r="23" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
         <v>12</v>
       </c>
-      <c r="J23">
-        <f>AVERAGE(J2:J14)</f>
+      <c r="M23">
+        <f>AVERAGE(M2:M14)</f>
         <v>2.2008466264275457</v>
+      </c>
+    </row>
+    <row r="30" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <v>95.987200000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <v>94.021199999999993</v>
+      </c>
+    </row>
+    <row r="32" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <v>64.846500000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <v>93.720200000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <v>89.3994</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>82.846500000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <v>81.807699999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <v>85.099699999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>91.972399999999993</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <v>92.323599999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>89.424300000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <v>85.177300000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <v>94.146799999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data and code update
</commit_message>
<xml_diff>
--- a/Data_Set/Raw/Bilan-dataSet.xlsx
+++ b/Data_Set/Raw/Bilan-dataSet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Nom</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Model prediction</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Interception</t>
+  </si>
+  <si>
+    <t>Corrélation</t>
   </si>
 </sst>
 </file>
@@ -101,9 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,16 +396,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C24" sqref="C24:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
     <col min="8" max="8" width="19.5546875" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
@@ -456,11 +470,11 @@
         <v>94.687248093435002</v>
       </c>
       <c r="L2">
-        <f>110-25*((E2/C2)/(F2/D2))</f>
+        <f t="shared" ref="L2:L14" si="0">110-25*((E2/C2)/(F2/D2))</f>
         <v>96.012349146745905</v>
       </c>
       <c r="M2">
-        <f>ABS(L2-G2)</f>
+        <f t="shared" ref="M2:M14" si="1">ABS(L2-G2)</f>
         <v>2.5149146745903295E-2</v>
       </c>
     </row>
@@ -490,11 +504,11 @@
         <v>94.959077458293095</v>
       </c>
       <c r="L3">
-        <f>110-25*((E3/C3)/(F3/D3))</f>
+        <f t="shared" si="0"/>
         <v>93.628005657708627</v>
       </c>
       <c r="M3">
-        <f>ABS(L3-G3)</f>
+        <f t="shared" si="1"/>
         <v>0.39319434229136618</v>
       </c>
     </row>
@@ -524,11 +538,11 @@
         <v>64.4323129265115</v>
       </c>
       <c r="L4">
-        <f>110-25*((E4/C4)/(F4/D4))</f>
+        <f t="shared" si="0"/>
         <v>52.849525696542891</v>
       </c>
       <c r="M4">
-        <f>ABS(L4-G4)</f>
+        <f t="shared" si="1"/>
         <v>11.996974303457115</v>
       </c>
     </row>
@@ -558,11 +572,11 @@
         <v>94.016962524455096</v>
       </c>
       <c r="L5">
-        <f>110-25*((E5/C5)/(F5/D5))</f>
+        <f t="shared" si="0"/>
         <v>93.674654736176279</v>
       </c>
       <c r="M5">
-        <f>ABS(L5-G5)</f>
+        <f t="shared" si="1"/>
         <v>4.5545263823726145E-2</v>
       </c>
     </row>
@@ -592,11 +606,11 @@
         <v>87.279647474527806</v>
       </c>
       <c r="L6">
-        <f>110-25*((E6/C6)/(F6/D6))</f>
+        <f t="shared" si="0"/>
         <v>86.976470911999485</v>
       </c>
       <c r="M6">
-        <f>ABS(L6-G6)</f>
+        <f t="shared" si="1"/>
         <v>2.4229290880005152</v>
       </c>
     </row>
@@ -626,11 +640,11 @@
         <v>85.653102188874399</v>
       </c>
       <c r="L7">
-        <f>110-25*((E7/C7)/(F7/D7))</f>
+        <f t="shared" si="0"/>
         <v>86.752771464848536</v>
       </c>
       <c r="M7">
-        <f>ABS(L7-G7)</f>
+        <f t="shared" si="1"/>
         <v>3.9062714648485297</v>
       </c>
     </row>
@@ -660,11 +674,11 @@
         <v>82.359686356429293</v>
       </c>
       <c r="L8">
-        <f>110-25*((E8/C8)/(F8/D8))</f>
+        <f t="shared" si="0"/>
         <v>81.946816127047242</v>
       </c>
       <c r="M8">
-        <f>ABS(L8-G8)</f>
+        <f t="shared" si="1"/>
         <v>0.13911612704724519</v>
       </c>
     </row>
@@ -694,11 +708,11 @@
         <v>85.242444694750503</v>
       </c>
       <c r="L9">
-        <f>110-25*((E9/C9)/(F9/D9))</f>
+        <f t="shared" si="0"/>
         <v>81.05399121673986</v>
       </c>
       <c r="M9">
-        <f>ABS(L9-G9)</f>
+        <f t="shared" si="1"/>
         <v>4.0457087832601388</v>
       </c>
     </row>
@@ -728,11 +742,11 @@
         <v>89.632383875928298</v>
       </c>
       <c r="L10">
-        <f>110-25*((E10/C10)/(F10/D10))</f>
+        <f t="shared" si="0"/>
         <v>91.91245791245791</v>
       </c>
       <c r="M10">
-        <f>ABS(L10-G10)</f>
+        <f t="shared" si="1"/>
         <v>5.99420875420833E-2</v>
       </c>
     </row>
@@ -762,11 +776,11 @@
         <v>89.348543617324793</v>
       </c>
       <c r="L11">
-        <f>110-25*((E11/C11)/(F11/D11))</f>
+        <f t="shared" si="0"/>
         <v>91.184471083183325</v>
       </c>
       <c r="M11">
-        <f>ABS(L11-G11)</f>
+        <f t="shared" si="1"/>
         <v>1.1391289168166736</v>
       </c>
     </row>
@@ -796,11 +810,11 @@
         <v>89.566795231854002</v>
       </c>
       <c r="L12">
-        <f>110-25*((E12/C12)/(F12/D12))</f>
+        <f t="shared" si="0"/>
         <v>88.397307614242123</v>
       </c>
       <c r="M12">
-        <f>ABS(L12-G12)</f>
+        <f t="shared" si="1"/>
         <v>1.0269923857578789</v>
       </c>
     </row>
@@ -830,11 +844,11 @@
         <v>89.590290789469705</v>
       </c>
       <c r="L13">
-        <f>110-25*((E13/C13)/(F13/D13))</f>
+        <f t="shared" si="0"/>
         <v>85.507562112623816</v>
       </c>
       <c r="M13">
-        <f>ABS(L13-G13)</f>
+        <f t="shared" si="1"/>
         <v>0.33026211262381366</v>
       </c>
     </row>
@@ -864,15 +878,15 @@
         <v>94.132884696235607</v>
       </c>
       <c r="L14">
-        <f>110-25*((E14/C14)/(F14/D14))</f>
+        <f t="shared" si="0"/>
         <v>91.067007878656895</v>
       </c>
       <c r="M14">
-        <f>ABS(L14-G14)</f>
+        <f t="shared" si="1"/>
         <v>3.0797921213431039</v>
       </c>
     </row>
-    <row r="23" spans="6:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
       <c r="L23" t="s">
         <v>12</v>
       </c>
@@ -881,72 +895,60 @@
         <v>2.2008466264275457</v>
       </c>
     </row>
-    <row r="30" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F30">
-        <v>95.987200000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F31">
-        <v>94.021199999999993</v>
-      </c>
-    </row>
-    <row r="32" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F32">
-        <v>64.846500000000006</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F33">
-        <v>93.720200000000006</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F34">
-        <v>89.3994</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F35">
-        <v>82.846500000000006</v>
-      </c>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F36">
-        <v>81.807699999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F37">
-        <v>85.099699999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F38">
-        <v>91.972399999999993</v>
-      </c>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F39">
-        <v>92.323599999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F40">
-        <v>89.424300000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F41">
-        <v>85.177300000000002</v>
-      </c>
-    </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F42">
-        <v>94.146799999999999</v>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>44.101038809999999</v>
+      </c>
+      <c r="D26">
+        <v>-24.604666720000001</v>
+      </c>
+      <c r="E26">
+        <v>-4575.9874201800003</v>
+      </c>
+      <c r="F26">
+        <v>2380.0554081800001</v>
+      </c>
+      <c r="G26">
+        <v>80.280442275973797</v>
+      </c>
+      <c r="H26">
+        <v>0.99422622728771903</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C24:H24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>